<commit_message>
Oak ffc ir (#420)
* Added initial release of PA0960_R0M0E0 of FFC-IR

* Update README.md

* Update README.md

* Updated DM0260 to revision R2M1E1

Missing pictures of new revision boards.

* Update README.md, with new revision status

* Added .STEP 3d model to 3D_Models folder

* Update README.md, added bold text where needed

* Update README.md, changed Altium designer from 22 to 23

* Added BOM files to DOCS

Added BOM files to projects:
- PA0960
- DM0260 for 1V0 and 1V2
- OAK-D-SR-PoE for EL2086 and EL6905

* Moved step files to DO

---------

Co-authored-by: Erol444 <erol123444@gmail.com>
</commit_message>
<xml_diff>
--- a/DM0260_OAK-FFC-CBA/Docs/FAB_1V0/Assembly Outputs/BOM/BOM-DM0260(Production_1V0).xlsx
+++ b/DM0260_OAK-FFC-CBA/Docs/FAB_1V0/Assembly Outputs/BOM/BOM-DM0260(Production_1V0).xlsx
@@ -1,25 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\DM0260\KingTop_Output_Files\Assembly Outputs\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60F913BE-A040-4605-92F3-BC31BB835647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="38340" windowHeight="20112"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{479A8F86-A8E0-4C65-A039-9816656EBF80}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-DM0260(Production_1V0)" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BOM-DM0260(Production_1V0)'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -156,22 +176,25 @@
     <t>F32R-1A7H1-11026</t>
   </si>
   <si>
+    <t>AC_PY003-OV9282_CON</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>FFC/FPC Connector, 33 Contact(s), 1 Row(s), Female, Right Angle, Surface Mount Terminal</t>
+  </si>
+  <si>
+    <t>Hirose</t>
+  </si>
+  <si>
     <t>FH26W-33S-0.3SHW(60)</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>FFC/FPC Connector, 33 Contact(s), 1 Row(s), Female, Right Angle, Surface Mount Terminal</t>
-  </si>
-  <si>
-    <t>Hirose</t>
-  </si>
-  <si>
-    <t>AC-PY004-IMX378</t>
-  </si>
-  <si>
-    <t>AC_PY004-IMX378_CON</t>
+    <t>AC-PY003-OV9282</t>
+  </si>
+  <si>
+    <t>CMP-005-000036-1</t>
   </si>
   <si>
     <t>1uH, 3.2A, 20%</t>
@@ -300,14 +323,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -360,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -368,14 +390,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pisarna">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -383,44 +408,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pisarna">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -448,14 +473,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -483,9 +525,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pisarna">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,171 +553,147 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B611330-B415-4D38-B8DC-734B60436246}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -924,305 +959,281 @@
         <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OAK-FFC-CBA (without 3d model)
</commit_message>
<xml_diff>
--- a/DM0260_OAK-FFC-CBA/Docs/FAB_1V0/Assembly Outputs/BOM/BOM-DM0260(Production_1V0).xlsx
+++ b/DM0260_OAK-FFC-CBA/Docs/FAB_1V0/Assembly Outputs/BOM/BOM-DM0260(Production_1V0).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\DM0260\KingTop_Output_Files\Assembly Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60F913BE-A040-4605-92F3-BC31BB835647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{132DDD17-286D-416D-9592-70A66ABA834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{479A8F86-A8E0-4C65-A039-9816656EBF80}"/>
+    <workbookView xWindow="40305" yWindow="1830" windowWidth="28800" windowHeight="17295" xr2:uid="{07AD1545-43F9-495F-99CF-C330E104BFFB}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-DM0260(Production_1V0)" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,24 @@
     <t>CAPC0402(1005)70_L, CAPC0402(1005)70_N</t>
   </si>
   <si>
+    <t>CL05B104KO5NFNC</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0402 10%</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>CAPC0402(1005)60_L</t>
+  </si>
+  <si>
+    <t>CMP-108-000002-6</t>
+  </si>
+  <si>
     <t>22uF 0603</t>
   </si>
   <si>
@@ -284,6 +302,36 @@
     <t>RC0402FR-0740K2L</t>
   </si>
   <si>
+    <t>RMCF0201FT10K0</t>
+  </si>
+  <si>
+    <t>R10, R11, R13</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1%  1/20W 0201</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RESC0201(0603)_L</t>
+  </si>
+  <si>
+    <t>CMP-009-00340-3</t>
+  </si>
+  <si>
+    <t>RC0402FR-071KL</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>CMP-013-000004-10</t>
+  </si>
+  <si>
     <t>TLV62080DSG</t>
   </si>
   <si>
@@ -318,6 +366,21 @@
   </si>
   <si>
     <t>TLV70028DCKT</t>
+  </si>
+  <si>
+    <t>24AA32A-I/MS</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>IC EEPROM 32K I2C 400KHZ 8MSOP Memory IC 32Kb (4K x 8) I²C 400kHz 900ns 8-MSOP</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>CMP-010-000010-1</t>
   </si>
 </sst>
 </file>
@@ -330,6 +393,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -382,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,9 +462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pisarna">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -438,7 +502,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pisarna">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -544,7 +608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pisarna">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -693,24 +757,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B611330-B415-4D38-B8DC-734B60436246}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB0011C-6A73-456B-A40A-A225A3AEDF3F}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="31.77734375" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -739,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -768,7 +832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -797,7 +861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -811,85 +875,85 @@
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>36</v>
@@ -904,7 +968,7 @@
         <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>39</v>
@@ -913,128 +977,128 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>63</v>
@@ -1049,7 +1113,7 @@
         <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>66</v>
@@ -1058,27 +1122,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>72</v>
@@ -1087,7 +1151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
@@ -1101,135 +1165,251 @@
         <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>